<commit_message>
updated classes and docs
</commit_message>
<xml_diff>
--- a/astroscheduler/config/TimeScheduleConfig.xlsx
+++ b/astroscheduler/config/TimeScheduleConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa368046\src\astroscheduler\data\sample_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa368046\src\astroscheduler\astroscheduler\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD7DFAF-F16F-4F0B-A033-C984210483B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD13D14D-2433-4AAE-A44B-5B5B28E8468D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{27BC9DC3-E900-43F2-B8D0-6E87A6A1ECD7}"/>
+    <workbookView xWindow="-76920" yWindow="-6390" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{27BC9DC3-E900-43F2-B8D0-6E87A6A1ECD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>WEE HOURS</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>TimeReference Absolute means the entry starts at the time of day Hour:Minute</t>
+  </si>
+  <si>
+    <t>ScheduleName</t>
+  </si>
+  <si>
+    <t>AstroSchedule</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F97FC5B-F882-4C6F-87FD-9B1B24A8C071}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -600,16 +606,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118592A6-78D1-4381-B65B-E6106D87DE35}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,6 +665,14 @@
       </c>
       <c r="B6" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -670,6 +684,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="70b5b486-62ca-446d-85b9-12534f89bcbd" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c56cb509-70af-4579-bdf7-5ea3b144dfb6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100249B0E9FE56F5948B602BA84FE20E907" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63949f8d055d5943d96d237c4ef691d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c56cb509-70af-4579-bdf7-5ea3b144dfb6" xmlns:ns3="70b5b486-62ca-446d-85b9-12534f89bcbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb804e7b5fa037c4b3c9872285b34489" ns2:_="" ns3:_="">
     <xsd:import namespace="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
@@ -904,27 +938,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="70b5b486-62ca-446d-85b9-12534f89bcbd" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c56cb509-70af-4579-bdf7-5ea3b144dfb6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7E3410-FB96-4A4F-BEF0-80AF9C94BD2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="70b5b486-62ca-446d-85b9-12534f89bcbd"/>
+    <ds:schemaRef ds:uri="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8BA42F-44F7-436B-8FF8-451BF8769D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D302D409-78E5-462F-B93A-F03EF0CB1A60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -943,25 +976,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8BA42F-44F7-436B-8FF8-451BF8769D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7E3410-FB96-4A4F-BEF0-80AF9C94BD2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="70b5b486-62ca-446d-85b9-12534f89bcbd"/>
-    <ds:schemaRef ds:uri="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{57443d00-af18-408c-9335-47b5de3ec9b9}" enabled="1" method="Privileged" siteId="{6e51e1ad-c54b-4b39-b598-0ffe9ae68fef}" contentBits="2" removed="0"/>

</xml_diff>